<commit_message>
TT Uploader formulae corrected
</commit_message>
<xml_diff>
--- a/TT_Uploader.xlsx
+++ b/TT_Uploader.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicko\Documents\GitHub\trackingtables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864611B8-C8A9-49B3-8A04-F0163E0A1C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742EC163-06F2-4983-B65F-7DE6C0EB1739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1039,8 +1039,14 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="E2" s="8" t="str">
+        <f>IF(D2="NULL",D2,"'"&amp;D2&amp;"'")</f>
+        <v>''</v>
+      </c>
+      <c r="F2" s="8" t="str">
+        <f>"('"&amp;A2&amp;"', "&amp;B2&amp;", "&amp;C2&amp;", "&amp;E2&amp;"),"</f>
+        <v>('', , , ''),</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>

</xml_diff>